<commit_message>
Updated readme with video
</commit_message>
<xml_diff>
--- a/Project Outputs for BusinessCard/BusinessCard.xlsx
+++ b/Project Outputs for BusinessCard/BusinessCard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium\Projects\BusinessCard\Project Outputs for BusinessCard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2603856-88F0-4E37-B685-A3EB408578EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68061BA2-7C2A-4FBE-BE52-63A2064B3A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="780" windowWidth="20865" windowHeight="11835" xr2:uid="{3054F4A1-A229-47E7-91CA-F1D7ED12BA90}"/>
+    <workbookView xWindow="2100" yWindow="1125" windowWidth="20865" windowHeight="11835" xr2:uid="{5AC6CBE3-2D91-4C45-9D3B-8D59A596F50A}"/>
   </bookViews>
   <sheets>
     <sheet name="BusinessCard" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="145">
   <si>
     <t>Comment</t>
   </si>
@@ -206,12 +206,21 @@
     <t>D5</t>
   </si>
   <si>
+    <t>VLMG1300-GS08</t>
+  </si>
+  <si>
+    <t>LED GREEN 0603 SMD</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>CMP-02520-000011-1</t>
+  </si>
+  <si>
     <t>TLMP1100-GS08</t>
   </si>
   <si>
-    <t>LED GREEN 0603 SMD</t>
-  </si>
-  <si>
     <t>DL2</t>
   </si>
   <si>
@@ -371,7 +380,7 @@
     <t>Chip Resistor, 100 Ohm, +/- 1%, 100 mW,-55 to 155 degC, 0603 (1608 Metric), RoHS, Tape and Ree</t>
   </si>
   <si>
-    <t>R6, R7, R8</t>
+    <t>R6, R7, R8, R12</t>
   </si>
   <si>
     <t>RESC1609X50X30ML8T20</t>
@@ -843,11 +852,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29B85F7-8360-41BB-A414-1F38375EB67B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C104DED-98DF-4C29-B27D-13A75B415FEA}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1107,208 +1116,208 @@
         <v>58</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="4">
+      <c r="C20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="3" t="s">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="4">
+      <c r="C22" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="3" t="s">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -1316,59 +1325,59 @@
     </row>
     <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="F24" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="F25" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
@@ -1376,87 +1385,107 @@
     </row>
     <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F27" s="4">
+      <c r="C28" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D28" s="3" t="s">
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F28" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F29" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="F30" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F30" s="4">
+      <c r="C31" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F31" s="4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="34" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="34" orientation="landscape" blackAndWhite="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>